<commit_message>
Adicao de texto DETONADO no arquivo
</commit_message>
<xml_diff>
--- a/PastaModelosBD/AgendaAulasParducci-2022-V02.xlsx
+++ b/PastaModelosBD/AgendaAulasParducci-2022-V02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonpflocal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2C27C0-A053-4038-97EE-8F80FB87F151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD264F3-3454-45B5-8CAE-4464DEBE94AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1" xr2:uid="{4EF25AD1-8FF2-4455-B1DD-8B4DF90E9049}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{4EF25AD1-8FF2-4455-B1DD-8B4DF90E9049}"/>
   </bookViews>
   <sheets>
     <sheet name="TURMAS" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
   <si>
     <t>MANHÃ</t>
   </si>
@@ -1317,6 +1317,9 @@
       <t xml:space="preserve">
 Aula 4,5,6 - Preencher a partir da coluna 3 no UpStream (usuário renato Yahoo) - MONTAR SPRINTS NO DOWNSTREAM</t>
     </r>
+  </si>
+  <si>
+    <t>DETONADO!!!!!</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1822,6 +1825,7 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,27 +2140,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CFE18D-6E4C-40AD-9FD5-B1D090358419}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2173,7 +2177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2187,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -2223,7 +2227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2233,7 +2237,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2253,7 +2257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2273,8 +2277,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="69" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2282,26 +2292,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79DBBC9-ED23-4144-AC1E-7BB2F491545B}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="48.44140625" customWidth="1"/>
-    <col min="4" max="4" width="47.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2318,7 +2328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2338,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="138.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2348,7 +2358,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -2368,7 +2378,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2378,7 +2388,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2398,7 +2408,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2432,22 +2442,22 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2464,7 +2474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -2474,7 +2484,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -2514,7 +2524,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2524,7 +2534,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2556,7 +2566,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>67</v>
       </c>
@@ -2566,7 +2576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2591,7 +2601,7 @@
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>61</v>
       </c>
@@ -2616,7 +2626,7 @@
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
@@ -2641,7 +2651,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2666,7 +2676,7 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2691,12 +2701,12 @@
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2704,7 +2714,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2726,23 +2736,23 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>106</v>
       </c>
@@ -2773,7 +2783,7 @@
       <c r="U3" s="54"/>
       <c r="V3" s="55"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>35</v>
       </c>
@@ -2798,7 +2808,7 @@
       <c r="U4" s="45"/>
       <c r="V4" s="46"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>36</v>
       </c>
@@ -2827,7 +2837,7 @@
       <c r="U5" s="48"/>
       <c r="V5" s="49"/>
     </row>
-    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>37</v>
       </c>
@@ -2856,7 +2866,7 @@
       <c r="U6" s="48"/>
       <c r="V6" s="49"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
@@ -2883,7 +2893,7 @@
       <c r="U7" s="48"/>
       <c r="V7" s="49"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
@@ -2912,7 +2922,7 @@
       <c r="U8" s="48"/>
       <c r="V8" s="49"/>
     </row>
-    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2941,7 +2951,7 @@
       <c r="U9" s="48"/>
       <c r="V9" s="49"/>
     </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K10" s="58" t="s">
         <v>100</v>
       </c>
@@ -2957,7 +2967,7 @@
       <c r="U10" s="48"/>
       <c r="V10" s="49"/>
     </row>
-    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>94</v>
       </c>
@@ -2986,7 +2996,7 @@
       <c r="U11" s="48"/>
       <c r="V11" s="49"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>35</v>
       </c>
@@ -3013,7 +3023,7 @@
       <c r="U12" s="48"/>
       <c r="V12" s="49"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>36</v>
       </c>
@@ -3042,7 +3052,7 @@
       <c r="U13" s="48"/>
       <c r="V13" s="49"/>
     </row>
-    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -3067,7 +3077,7 @@
       <c r="U14" s="48"/>
       <c r="V14" s="49"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>42</v>
       </c>
@@ -3094,7 +3104,7 @@
       <c r="U15" s="48"/>
       <c r="V15" s="49"/>
     </row>
-    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>37</v>
       </c>
@@ -3123,7 +3133,7 @@
       <c r="U16" s="48"/>
       <c r="V16" s="49"/>
     </row>
-    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -3146,8 +3156,8 @@
       <c r="U17" s="51"/>
       <c r="V17" s="52"/>
     </row>
-    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>98</v>
       </c>
@@ -3176,7 +3186,7 @@
       <c r="U19" s="54"/>
       <c r="V19" s="55"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>35</v>
       </c>
@@ -3201,7 +3211,7 @@
       <c r="U20" s="45"/>
       <c r="V20" s="46"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>36</v>
       </c>
@@ -3230,7 +3240,7 @@
       <c r="U21" s="48"/>
       <c r="V21" s="49"/>
     </row>
-    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>37</v>
       </c>
@@ -3259,7 +3269,7 @@
       <c r="U22" s="48"/>
       <c r="V22" s="49"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>42</v>
       </c>
@@ -3286,7 +3296,7 @@
       <c r="U23" s="48"/>
       <c r="V23" s="49"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>36</v>
       </c>
@@ -3315,7 +3325,7 @@
       <c r="U24" s="48"/>
       <c r="V24" s="49"/>
     </row>
-    <row r="25" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>37</v>
       </c>
@@ -3344,7 +3354,7 @@
       <c r="U25" s="48"/>
       <c r="V25" s="49"/>
     </row>
-    <row r="26" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K26" s="47" t="s">
         <v>105</v>
       </c>
@@ -3360,7 +3370,7 @@
       <c r="U26" s="48"/>
       <c r="V26" s="49"/>
     </row>
-    <row r="27" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>55</v>
       </c>
@@ -3387,7 +3397,7 @@
       <c r="U27" s="48"/>
       <c r="V27" s="49"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>35</v>
       </c>
@@ -3412,7 +3422,7 @@
       <c r="U28" s="48"/>
       <c r="V28" s="49"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>36</v>
       </c>
@@ -3439,7 +3449,7 @@
       <c r="U29" s="48"/>
       <c r="V29" s="49"/>
     </row>
-    <row r="30" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>37</v>
       </c>
@@ -3466,7 +3476,7 @@
       <c r="U30" s="51"/>
       <c r="V30" s="52"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>42</v>
       </c>
@@ -3479,7 +3489,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>36</v>
       </c>
@@ -3494,7 +3504,7 @@
       <c r="H32" s="34"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>37</v>
       </c>
@@ -3524,17 +3534,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -3542,7 +3552,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3550,7 +3560,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>

</xml_diff>